<commit_message>
concept draft and first tries to set up logging module
Signed-off-by: elgustov <max.may8@web.de>
</commit_message>
<xml_diff>
--- a/src/schedule.xlsx
+++ b/src/schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Max\Documents\Master IIS\AMOS\amos2022ws01-firmware-scraper\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E625D688-550C-4B1F-AFEB-9155C227E6B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52B3523C-88FD-4833-9928-2BCD3678756A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-4990" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-36440" yWindow="-2920" windowWidth="28800" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>Unnamed: 0</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Vendor</t>
   </si>
@@ -449,19 +446,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -474,59 +471,47 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2">
+        <v>44881</v>
+      </c>
+      <c r="D2" s="2">
+        <v>44881</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2" s="2">
-        <v>44879</v>
-      </c>
-      <c r="E2" s="2">
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3" s="2">
         <v>44881</v>
       </c>
+      <c r="D3" s="2">
+        <v>44884</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="C3">
-        <v>3</v>
-      </c>
-      <c r="D3" s="2">
-        <v>44879</v>
-      </c>
-      <c r="E3" s="2">
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4" s="2">
         <v>44881</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4">
-        <v>5</v>
-      </c>
       <c r="D4" s="2">
-        <v>44879</v>
-      </c>
-      <c r="E4" s="2">
-        <v>44881</v>
+        <v>44886</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finalized scheduler/logger connection to core/Vendors
Signed-off-by: elgustov <max.may8@web.de>
</commit_message>
<xml_diff>
--- a/src/schedule.xlsx
+++ b/src/schedule.xlsx
@@ -1,42 +1,76 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Max\Documents\Master IIS\AMOS\amos2022ws01-firmware-scraper\src\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D19AA2B0-18AD-4613-B447-8F25C3767817}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="3040" yWindow="3040" windowWidth="28800" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>Vendor</t>
+  </si>
+  <si>
+    <t>Intervall</t>
+  </si>
+  <si>
+    <t>Last_update</t>
+  </si>
+  <si>
+    <t>Next_update</t>
+  </si>
+  <si>
+    <t>Siemens</t>
+  </si>
+  <si>
+    <t>Asus</t>
+  </si>
+  <si>
+    <t>Schneider</t>
+  </si>
+  <si>
+    <t>AVM</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
-    <numFmt numFmtId="166" formatCode="yyyy-mm-dd"/>
-    <numFmt numFmtId="167" formatCode="YYYY-MM-DD"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -51,95 +85,45 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -427,103 +411,87 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7265625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Vendor</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Intervall</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Last_update</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Next_update</t>
-        </is>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Siemens</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
         <v>100</v>
       </c>
-      <c r="C2" s="2" t="n">
+      <c r="C2" s="2">
         <v>44894</v>
       </c>
-      <c r="D2" s="3" t="n">
+      <c r="D2" s="3">
         <v>44993</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Asus</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
         <v>100</v>
       </c>
-      <c r="C3" s="2" t="n">
+      <c r="C3" s="2">
         <v>44893</v>
       </c>
-      <c r="D3" s="3" t="n">
+      <c r="D3" s="3">
         <v>44896</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Schneider</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
         <v>0</v>
       </c>
-      <c r="C4" s="3" t="n">
+      <c r="C4" s="3">
         <v>44894</v>
       </c>
-      <c r="D4" s="2" t="n">
+      <c r="D4" s="2">
         <v>44894</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>AVM</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>10</v>
-      </c>
-      <c r="C5" s="2" t="n">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5" s="3">
         <v>44894</v>
       </c>
-      <c r="D5" s="3" t="n">
-        <v>44904</v>
+      <c r="D5" s="2">
+        <v>44894</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improved logic between core and scheduler
Signed-off-by: elgustov <max.may8@web.de>
</commit_message>
<xml_diff>
--- a/src/schedule.xlsx
+++ b/src/schedule.xlsx
@@ -1,76 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Max\Documents\Master IIS\AMOS\amos2022ws01-firmware-scraper\src\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D19AA2B0-18AD-4613-B447-8F25C3767817}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="3040" yWindow="3040" windowWidth="28800" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>Vendor</t>
-  </si>
-  <si>
-    <t>Intervall</t>
-  </si>
-  <si>
-    <t>Last_update</t>
-  </si>
-  <si>
-    <t>Next_update</t>
-  </si>
-  <si>
-    <t>Siemens</t>
-  </si>
-  <si>
-    <t>Asus</t>
-  </si>
-  <si>
-    <t>Schneider</t>
-  </si>
-  <si>
-    <t>AVM</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="166" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="167" formatCode="YYYY-MM-DD"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -85,45 +51,95 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -411,87 +427,103 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="3" max="3" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.7265625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Vendor</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Intervall</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Last_update</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Next_update</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Siemens</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>100</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>44894</v>
+      </c>
+      <c r="D2" s="3" t="n">
+        <v>44993</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Asus</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>100</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>44893</v>
+      </c>
+      <c r="D3" s="3" t="n">
+        <v>44896</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Schneider</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
+      <c r="C4" s="3" t="n">
+        <v>44895</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>44895</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2">
-        <v>100</v>
-      </c>
-      <c r="C2" s="2">
-        <v>44894</v>
-      </c>
-      <c r="D2" s="3">
-        <v>44993</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3">
-        <v>100</v>
-      </c>
-      <c r="C3" s="2">
-        <v>44893</v>
-      </c>
-      <c r="D3" s="3">
-        <v>44896</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4">
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>AVM</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
         <v>0</v>
       </c>
-      <c r="C4" s="3">
-        <v>44894</v>
-      </c>
-      <c r="D4" s="2">
-        <v>44894</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5" s="3">
-        <v>44894</v>
-      </c>
-      <c r="D5" s="2">
-        <v>44894</v>
+      <c r="C5" s="3" t="n">
+        <v>44895</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>44895</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Integrated scheduler.py into core.py - Initializing Vendorclasses directly from xlsx file without dict
Signed-off-by: elgustov <max.may8@web.de>
</commit_message>
<xml_diff>
--- a/src/schedule.xlsx
+++ b/src/schedule.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,6 +461,16 @@
           <t>Next_update</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Vendor_class</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>max_products</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -477,6 +487,8 @@
       <c r="D2" s="3" t="n">
         <v>44993</v>
       </c>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -491,8 +503,10 @@
         <v>44893</v>
       </c>
       <c r="D3" s="3" t="n">
-        <v>44896</v>
-      </c>
+        <v>45261</v>
+      </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -504,10 +518,18 @@
         <v>0</v>
       </c>
       <c r="C4" s="3" t="n">
-        <v>44895</v>
+        <v>44899</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>44895</v>
+        <v>44899</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>SchneiderElectricScraper</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="5">
@@ -520,11 +542,39 @@
         <v>0</v>
       </c>
       <c r="C5" s="3" t="n">
-        <v>44895</v>
+        <v>44899</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>44895</v>
-      </c>
+        <v>44899</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>AVMScraper</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Synology</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="3" t="n">
+        <v>44899</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>44899</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Synology_scraper</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
AVM is last vendor, as max_products doenst reduce testing time.
</commit_message>
<xml_diff>
--- a/src/schedule.xlsx
+++ b/src/schedule.xlsx
@@ -1,42 +1,94 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kiril/Documents/Dokumente-onefive/00_Self/Master/Semester_5/AMOS/amos2022ws01-firmware-scraper/src/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78B02D99-5E8D-5341-8DE1-6977F91C143C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="23500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+  <si>
+    <t>Vendor</t>
+  </si>
+  <si>
+    <t>Intervall</t>
+  </si>
+  <si>
+    <t>Last_update</t>
+  </si>
+  <si>
+    <t>Next_update</t>
+  </si>
+  <si>
+    <t>Vendor_class</t>
+  </si>
+  <si>
+    <t>max_products</t>
+  </si>
+  <si>
+    <t>Siemens</t>
+  </si>
+  <si>
+    <t>Asus</t>
+  </si>
+  <si>
+    <t>Schneider</t>
+  </si>
+  <si>
+    <t>SchneiderElectricScraper</t>
+  </si>
+  <si>
+    <t>AVM</t>
+  </si>
+  <si>
+    <t>AVMScraper</t>
+  </si>
+  <si>
+    <t>Synology</t>
+  </si>
+  <si>
+    <t>SynologyScraper</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
-    <numFmt numFmtId="166" formatCode="yyyy-mm-dd"/>
-    <numFmt numFmtId="167" formatCode="YYYY-MM-DD"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -51,95 +103,45 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -427,154 +429,116 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Vendor</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Intervall</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Last_update</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Next_update</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Vendor_class</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>max_products</t>
-        </is>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Siemens</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
         <v>100</v>
       </c>
-      <c r="C2" s="2" t="n">
+      <c r="C2" s="2">
         <v>44894</v>
       </c>
-      <c r="D2" s="3" t="n">
+      <c r="D2" s="3">
         <v>44993</v>
       </c>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Asus</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3">
         <v>100</v>
       </c>
-      <c r="C3" s="2" t="n">
+      <c r="C3" s="2">
         <v>44893</v>
       </c>
-      <c r="D3" s="3" t="n">
+      <c r="D3" s="3">
         <v>45261</v>
       </c>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Schneider</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
         <v>0</v>
       </c>
-      <c r="C4" s="3" t="n">
+      <c r="C4" s="3">
         <v>44899</v>
       </c>
-      <c r="D4" s="2" t="n">
+      <c r="D4" s="2">
         <v>44899</v>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>SchneiderElectricScraper</t>
-        </is>
-      </c>
-      <c r="F4" t="n">
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4">
         <v>10</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>AVM</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5">
         <v>0</v>
       </c>
-      <c r="C5" s="3" t="n">
+      <c r="C5" s="3">
         <v>44899</v>
       </c>
-      <c r="D5" s="2" t="n">
+      <c r="D5" s="2">
         <v>44899</v>
       </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>AVMScraper</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr"/>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Synology</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>0</v>
-      </c>
-      <c r="C6" s="3" t="n">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6">
+        <v>100</v>
+      </c>
+      <c r="C6" s="3">
         <v>44899</v>
       </c>
-      <c r="D6" s="2" t="n">
+      <c r="D6" s="2">
         <v>44899</v>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Synology_scraper</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr"/>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Fix for Synology class in schedule.xlsx
Signed-off-by: elgustov <max.may8@web.de>
</commit_message>
<xml_diff>
--- a/src/schedule.xlsx
+++ b/src/schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kiril/Documents/Dokumente-onefive/00_Self/Master/Semester_5/AMOS/amos2022ws01-firmware-scraper/src/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Max\Documents\Master IIS\AMOS\amos2022ws01-firmware-scraper\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78B02D99-5E8D-5341-8DE1-6977F91C143C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F61994D-C17C-40B6-A874-BDAAFC4F686D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="23500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16320" yWindow="6945" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -433,12 +433,15 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="17.7265625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -458,7 +461,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -472,7 +475,7 @@
         <v>44993</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -486,18 +489,18 @@
         <v>45261</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
-      <c r="C4" s="3">
-        <v>44899</v>
-      </c>
-      <c r="D4" s="2">
-        <v>44899</v>
+      <c r="C4" s="2">
+        <v>44901</v>
+      </c>
+      <c r="D4" s="3">
+        <v>45266</v>
       </c>
       <c r="E4" t="s">
         <v>9</v>
@@ -506,38 +509,38 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
-      <c r="C5" s="3">
-        <v>44899</v>
-      </c>
-      <c r="D5" s="2">
-        <v>44899</v>
+      <c r="C5" s="2">
+        <v>44902</v>
+      </c>
+      <c r="D5" s="3">
+        <v>44902</v>
       </c>
       <c r="E5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6" s="3">
+        <v>44902</v>
+      </c>
+      <c r="D6" s="2">
+        <v>44902</v>
+      </c>
+      <c r="E6" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6">
-        <v>100</v>
-      </c>
-      <c r="C6" s="3">
-        <v>44899</v>
-      </c>
-      <c r="D6" s="2">
-        <v>44899</v>
-      </c>
-      <c r="E6" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TP-Link: prepare integration into core
Signed-off-by: Leon Schäffer <l.schaeffer@campus.tu-berlin.de>
</commit_message>
<xml_diff>
--- a/src/schedule.xlsx
+++ b/src/schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Max\Documents\Master IIS\AMOS\amos2022ws01-firmware-scraper\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Leon/Library/Mobile Documents/com~apple~CloudDocs/TUB/22_WS/AMOS/repo/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F61994D-C17C-40B6-A874-BDAAFC4F686D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9395A48-B9DF-8B43-8B63-0F96412E1E22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="6945" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34760" yWindow="500" windowWidth="16440" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Vendor</t>
   </si>
@@ -62,6 +62,12 @@
   </si>
   <si>
     <t>SynologyScraper</t>
+  </si>
+  <si>
+    <t>TP-Link</t>
+  </si>
+  <si>
+    <t>TPLinkScraper</t>
   </si>
 </sst>
 </file>
@@ -430,18 +436,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -461,7 +468,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -475,7 +482,7 @@
         <v>44993</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -489,7 +496,7 @@
         <v>45261</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -500,7 +507,7 @@
         <v>44901</v>
       </c>
       <c r="D4" s="3">
-        <v>45266</v>
+        <v>45261</v>
       </c>
       <c r="E4" t="s">
         <v>9</v>
@@ -509,7 +516,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -520,13 +527,13 @@
         <v>44902</v>
       </c>
       <c r="D5" s="3">
-        <v>44902</v>
+        <v>45261</v>
       </c>
       <c r="E5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -536,11 +543,31 @@
       <c r="C6" s="3">
         <v>44902</v>
       </c>
-      <c r="D6" s="2">
-        <v>44902</v>
+      <c r="D6" s="3">
+        <v>45261</v>
       </c>
       <c r="E6" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7" s="3">
+        <v>44902</v>
+      </c>
+      <c r="D7" s="3">
+        <v>44902</v>
+      </c>
+      <c r="E7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Schneider: increase timeout to scrape result pages to 30s
Signed-off-by: Leon Schäffer <l.schaeffer@campus.tu-berlin.de>
</commit_message>
<xml_diff>
--- a/src/schedule.xlsx
+++ b/src/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Leon/Library/Mobile Documents/com~apple~CloudDocs/TUB/22_WS/AMOS/repo/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9395A48-B9DF-8B43-8B63-0F96412E1E22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEA479C5-9814-8C45-9D92-DE7FF68C0610}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34760" yWindow="500" windowWidth="16440" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -439,11 +439,12 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="3" max="3" width="25.1640625" customWidth="1"/>
     <col min="4" max="4" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="30" customWidth="1"/>
   </cols>
@@ -507,7 +508,7 @@
         <v>44901</v>
       </c>
       <c r="D4" s="3">
-        <v>45261</v>
+        <v>44902</v>
       </c>
       <c r="E4" t="s">
         <v>9</v>
@@ -527,7 +528,7 @@
         <v>44902</v>
       </c>
       <c r="D5" s="3">
-        <v>45261</v>
+        <v>44902</v>
       </c>
       <c r="E5" t="s">
         <v>11</v>
@@ -544,7 +545,7 @@
         <v>44902</v>
       </c>
       <c r="D6" s="3">
-        <v>45261</v>
+        <v>44902</v>
       </c>
       <c r="E6" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
get docker to run for new release
</commit_message>
<xml_diff>
--- a/src/schedule.xlsx
+++ b/src/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kiril/Documents/Dokumente-onefive/00_Self/Master/Semester_5/AMOS/amos2022ws01-firmware-scraper/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DDA5A39-664F-834D-A27C-D1926444EA13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4E16F13-A780-CD44-B659-5E22C630D523}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="23500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -439,12 +439,13 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -531,6 +532,9 @@
       <c r="E5" t="s">
         <v>15</v>
       </c>
+      <c r="F5">
+        <v>10</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -548,6 +552,9 @@
       <c r="E6" t="s">
         <v>13</v>
       </c>
+      <c r="F6">
+        <v>10</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -564,6 +571,9 @@
       </c>
       <c r="E7" t="s">
         <v>11</v>
+      </c>
+      <c r="F7">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rockwell first working version
Signed-off-by: elgustov <max.may8@web.de>
</commit_message>
<xml_diff>
--- a/src/schedule.xlsx
+++ b/src/schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Max\Documents\Master IIS\AMOS\amos2022ws01-firmware-scraper\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F61994D-C17C-40B6-A874-BDAAFC4F686D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8A308FB-9918-41E7-8693-4FDC85B76CFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="6945" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -433,7 +433,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -500,7 +500,7 @@
         <v>44901</v>
       </c>
       <c r="D4" s="3">
-        <v>45266</v>
+        <v>44901</v>
       </c>
       <c r="E4" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Swisscom: integrate into core
Signed-off-by: Leon Schäffer <l.schaeffer@campus.tu-berlin.de>
</commit_message>
<xml_diff>
--- a/src/schedule.xlsx
+++ b/src/schedule.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Leon/Library/Mobile Documents/com~apple~CloudDocs/TUB/22_WS/AMOS/repo/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEA479C5-9814-8C45-9D92-DE7FF68C0610}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F45817E-18F3-BD43-9A9B-A67332259A62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34760" yWindow="500" windowWidth="16440" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Vendor</t>
   </si>
@@ -68,6 +68,12 @@
   </si>
   <si>
     <t>TPLinkScraper</t>
+  </si>
+  <si>
+    <t>Swisscom</t>
+  </si>
+  <si>
+    <t>SwisscomScraper</t>
   </si>
 </sst>
 </file>
@@ -90,6 +96,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -436,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -508,7 +515,7 @@
         <v>44901</v>
       </c>
       <c r="D4" s="3">
-        <v>44902</v>
+        <v>45261</v>
       </c>
       <c r="E4" t="s">
         <v>9</v>
@@ -528,7 +535,7 @@
         <v>44902</v>
       </c>
       <c r="D5" s="3">
-        <v>44902</v>
+        <v>45261</v>
       </c>
       <c r="E5" t="s">
         <v>11</v>
@@ -545,7 +552,7 @@
         <v>44902</v>
       </c>
       <c r="D6" s="3">
-        <v>44902</v>
+        <v>45261</v>
       </c>
       <c r="E6" t="s">
         <v>13</v>
@@ -553,7 +560,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -562,12 +569,29 @@
         <v>44902</v>
       </c>
       <c r="D7" s="3">
+        <v>44927</v>
+      </c>
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8">
+        <v>100</v>
+      </c>
+      <c r="C8" s="3">
         <v>44902</v>
       </c>
-      <c r="E7" t="s">
+      <c r="D8" s="3">
+        <v>45261</v>
+      </c>
+      <c r="E8" t="s">
         <v>15</v>
       </c>
-      <c r="F7">
+      <c r="F8">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Zyxel, ABB and Trendnet to Scheduler
Signed-off-by: oliver99str <oliver.strauch@campus.tu-berlin.de>
</commit_message>
<xml_diff>
--- a/src/schedule.xlsx
+++ b/src/schedule.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Leon/Library/Mobile Documents/com~apple~CloudDocs/TUB/22_WS/AMOS/repo/src/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F45817E-18F3-BD43-9A9B-A67332259A62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34760" yWindow="500" windowWidth="16440" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Vendor</t>
   </si>
@@ -64,27 +58,56 @@
     <t>SynologyScraper</t>
   </si>
   <si>
+    <t>Swisscom</t>
+  </si>
+  <si>
+    <t>SwisscomScraper</t>
+  </si>
+  <si>
+    <t>Zyxel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-12-07
+2022-12-07
+</t>
+  </si>
+  <si>
+    <t>ZyxelScraper</t>
+  </si>
+  <si>
+    <t>ABB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-12-07
+2022-12-07
+"
+</t>
+  </si>
+  <si>
+    <t>ABBScraper</t>
+  </si>
+  <si>
+    <t>Trendnet</t>
+  </si>
+  <si>
+    <t>TrendnetScraper</t>
+  </si>
+  <si>
     <t>TP-Link</t>
   </si>
   <si>
     <t>TPLinkScraper</t>
-  </si>
-  <si>
-    <t>Swisscom</t>
-  </si>
-  <si>
-    <t>SwisscomScraper</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="165" formatCode="yyyy-mm-dd hh:mm:ss"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -95,6 +118,13 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -107,7 +137,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -117,42 +147,77 @@
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
       </right>
       <top style="thin">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+  <cellXfs count="13">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="165" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -163,10 +228,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -204,69 +269,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -290,54 +357,53 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
                 <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
+                <a:tint val="51000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
+                <a:tint val="15000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
+                <a:tint val="94000"/>
                 <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
+              <a:shade val="9500"/>
               <a:satMod val="105000"/>
             </a:schemeClr>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -347,7 +413,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -356,7 +422,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -365,7 +431,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -373,10 +439,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -405,7 +471,7 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
+                <a:tint val="20000"/>
                 <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
@@ -418,13 +484,12 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
                 <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
                 <a:satMod val="200000"/>
               </a:schemeClr>
             </a:gs>
@@ -442,160 +507,225 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="25.1640625" customWidth="1"/>
-    <col min="4" max="4" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30" customWidth="1"/>
+    <col min="1" max="1" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="12" width="25.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="12" width="17.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="10" width="30.005" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+      <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="5">
         <v>100</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="6">
         <v>44894</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="7">
         <v>44993</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="E2" s="4"/>
+      <c r="F2" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+      <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="5">
         <v>100</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="6">
         <v>44893</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="7">
         <v>45261</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="E3" s="4"/>
+      <c r="F3" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+      <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="5">
         <v>0</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="6">
         <v>44901</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="7">
         <v>45261</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="5">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+      <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="5">
         <v>0</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="6">
         <v>44902</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="7">
         <v>45261</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="F5" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+      <c r="A6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="5">
         <v>0</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="7">
         <v>44902</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="7">
         <v>45261</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="F6" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+      <c r="A7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="5">
+        <v>0</v>
+      </c>
+      <c r="C7" s="7">
+        <v>44902</v>
+      </c>
+      <c r="D7" s="7">
+        <v>44927</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+      <c r="A8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B7">
+      <c r="B8" s="8">
         <v>0</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C8" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="9">
+        <v>44927</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+      <c r="A9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="8">
+        <v>0</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="9">
+        <v>44927</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+      <c r="A10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="8">
+        <v>0</v>
+      </c>
+      <c r="C10" s="9">
         <v>44902</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D10" s="9">
         <v>44927</v>
       </c>
-      <c r="E7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8">
+      <c r="E10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+      <c r="A11" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="5">
         <v>100</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C11" s="7">
         <v>44902</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D11" s="7">
         <v>45261</v>
       </c>
-      <c r="E8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8">
+      <c r="E11" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="5">
         <v>20</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
schedule file as in main
Signed-off-by: elgustov <max.may8@web.de>
</commit_message>
<xml_diff>
--- a/src/schedule.xlsx
+++ b/src/schedule.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Max\Documents\Master IIS\AMOS\amos2022ws01-firmware-scraper\src\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87F0DACF-40D0-4959-A343-4A40D377B7BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Vendor</t>
   </si>
@@ -64,21 +58,56 @@
     <t>SynologyScraper</t>
   </si>
   <si>
-    <t>Rockwell</t>
-  </si>
-  <si>
-    <t>RockwellScraper</t>
+    <t>Swisscom</t>
+  </si>
+  <si>
+    <t>SwisscomScraper</t>
+  </si>
+  <si>
+    <t>Zyxel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-12-07
+2022-12-07
+</t>
+  </si>
+  <si>
+    <t>ZyxelScraper</t>
+  </si>
+  <si>
+    <t>ABB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-12-07
+2022-12-07
+"
+</t>
+  </si>
+  <si>
+    <t>ABBScraper</t>
+  </si>
+  <si>
+    <t>Trendnet</t>
+  </si>
+  <si>
+    <t>TrendnetScraper</t>
+  </si>
+  <si>
+    <t>TP-Link</t>
+  </si>
+  <si>
+    <t>TPLinkScraper</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="165" formatCode="yyyy-mm-dd hh:mm:ss"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -89,7 +118,15 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -100,7 +137,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -110,42 +147,77 @@
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
       </right>
       <top style="thin">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+  <cellXfs count="13">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="165" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -156,10 +228,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -197,69 +269,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -283,54 +357,53 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
                 <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
+                <a:tint val="51000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
+                <a:tint val="15000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
+                <a:tint val="94000"/>
                 <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
+              <a:shade val="9500"/>
               <a:satMod val="105000"/>
             </a:schemeClr>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -340,7 +413,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -349,7 +422,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -358,7 +431,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -366,10 +439,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -398,7 +471,7 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
+                <a:tint val="20000"/>
                 <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
@@ -411,13 +484,12 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
                 <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
                 <a:satMod val="200000"/>
               </a:schemeClr>
             </a:gs>
@@ -435,139 +507,225 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="4" width="17.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="12" width="25.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="12" width="17.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="10" width="30.005" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+      <c r="A2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="5">
+        <v>100</v>
+      </c>
+      <c r="C2" s="6">
+        <v>44894</v>
+      </c>
+      <c r="D2" s="7">
+        <v>44993</v>
+      </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+      <c r="A3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="5">
+        <v>100</v>
+      </c>
+      <c r="C3" s="6">
+        <v>44893</v>
+      </c>
+      <c r="D3" s="7">
+        <v>45261</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+      <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B2">
+      <c r="B4" s="5">
         <v>0</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C4" s="6">
         <v>44901</v>
       </c>
-      <c r="D2" s="3">
-        <v>44901</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="D4" s="7">
+        <v>45261</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F2">
+      <c r="F4" s="5">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+      <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B3">
+      <c r="B5" s="5">
         <v>0</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C5" s="6">
         <v>44902</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D5" s="7">
+        <v>45261</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+      <c r="A6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="5">
+        <v>0</v>
+      </c>
+      <c r="C6" s="7">
         <v>44902</v>
       </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="D6" s="7">
+        <v>45261</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+      <c r="A7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B4">
+      <c r="B7" s="5">
         <v>0</v>
       </c>
-      <c r="C4" s="3">
-        <v>44934</v>
-      </c>
-      <c r="D4" s="3">
-        <v>44935</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="C7" s="7">
+        <v>44902</v>
+      </c>
+      <c r="D7" s="7">
+        <v>44927</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5">
+      <c r="F7" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+      <c r="A8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="8">
+        <v>0</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="9">
+        <v>44927</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+      <c r="A9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="8">
+        <v>0</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="9">
+        <v>44927</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+      <c r="A10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="8">
+        <v>0</v>
+      </c>
+      <c r="C10" s="9">
+        <v>44902</v>
+      </c>
+      <c r="D10" s="9">
+        <v>44927</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+      <c r="A11" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="5">
         <v>100</v>
       </c>
-      <c r="C5" s="2">
-        <v>44894</v>
-      </c>
-      <c r="D5" s="3">
-        <v>44993</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6">
-        <v>100</v>
-      </c>
-      <c r="C6" s="2">
-        <v>44893</v>
-      </c>
-      <c r="D6" s="3">
+      <c r="C11" s="7">
+        <v>44902</v>
+      </c>
+      <c r="D11" s="7">
         <v>45261</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7" s="3">
-        <v>44902</v>
-      </c>
-      <c r="D7" s="2">
-        <v>44902</v>
-      </c>
-      <c r="E7" t="s">
-        <v>13</v>
+      <c r="E11" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="5">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Rockwell to schedule file
Signed-off-by: elgustov <max.may8@web.de>
</commit_message>
<xml_diff>
--- a/src/schedule.xlsx
+++ b/src/schedule.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25831"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Max\Documents\Master IIS\AMOS\amos2022ws01-firmware-scraper\src\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F89FF55-6657-45EF-829A-A37F2D5572C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Vendor</t>
   </si>
@@ -98,14 +104,20 @@
   <si>
     <t>TPLinkScraper</t>
   </si>
+  <si>
+    <t>Rockwell</t>
+  </si>
+  <si>
+    <t>RockwellScraper</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
-    <numFmt numFmtId="165" formatCode="yyyy-mm-dd hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -171,53 +183,42 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+  <cellXfs count="9">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="165" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -228,10 +229,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -269,71 +270,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -361,7 +362,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -384,11 +385,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -397,13 +398,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -413,7 +414,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -422,7 +423,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -431,7 +432,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -439,10 +440,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -507,25 +508,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="12" width="25.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="12" width="17.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="10" width="30.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.54296875" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.1796875" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7265625" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.54296875" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
+    <row r="1" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -545,184 +548,191 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="4">
         <v>100</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="5">
         <v>44894</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="6">
         <v>44993</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="8"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="4" t="s">
+    </row>
+    <row r="3" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <v>100</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="5">
         <v>44893</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="6">
         <v>45261</v>
       </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="8"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="4" t="s">
+    </row>
+    <row r="4" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="5">
-        <v>0</v>
-      </c>
-      <c r="C4" s="6">
+      <c r="B4" s="4">
+        <v>0</v>
+      </c>
+      <c r="C4" s="5">
         <v>44901</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="6">
         <v>45261</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="4">
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="5">
-        <v>0</v>
-      </c>
-      <c r="C5" s="6">
+      <c r="B5" s="4">
+        <v>0</v>
+      </c>
+      <c r="C5" s="5">
         <v>44902</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="6">
         <v>45261</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="8"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="4" t="s">
+    </row>
+    <row r="6" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="5">
-        <v>0</v>
-      </c>
-      <c r="C6" s="7">
+      <c r="B6" s="4">
+        <v>0</v>
+      </c>
+      <c r="C6" s="6">
         <v>44902</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="6">
         <v>45261</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="8"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
-      <c r="A7" s="4" t="s">
+    </row>
+    <row r="7" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="5">
-        <v>0</v>
-      </c>
-      <c r="C7" s="7">
+      <c r="B7" s="4">
+        <v>0</v>
+      </c>
+      <c r="C7" s="6">
         <v>44902</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="6">
         <v>44927</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="8"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
-      <c r="A8" s="4" t="s">
+    </row>
+    <row r="8" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="8">
-        <v>0</v>
-      </c>
-      <c r="C8" s="9" t="s">
+      <c r="B8" s="7">
+        <v>0</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="8">
         <v>44927</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="8"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
-      <c r="A9" s="4" t="s">
+    </row>
+    <row r="9" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="8">
-        <v>0</v>
-      </c>
-      <c r="C9" s="9" t="s">
+      <c r="B9" s="7">
+        <v>0</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="8">
         <v>44927</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="8"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
-      <c r="A10" s="4" t="s">
+    </row>
+    <row r="10" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="8">
-        <v>0</v>
-      </c>
-      <c r="C10" s="9">
+      <c r="B10" s="7">
+        <v>0</v>
+      </c>
+      <c r="C10" s="8">
         <v>44902</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="8">
         <v>44927</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="8"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
-      <c r="A11" s="4" t="s">
+    </row>
+    <row r="11" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="4">
         <v>100</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="6">
         <v>44902</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="6">
         <v>45261</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" t="s">
         <v>25</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="4">
         <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="7">
+        <v>0</v>
+      </c>
+      <c r="C12" s="6">
+        <v>44934</v>
+      </c>
+      <c r="D12" s="6">
+        <v>44935</v>
+      </c>
+      <c r="E12" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed .xlsx file back to main
Signed-off-by: elgustov <max.may8@web.de>
</commit_message>
<xml_diff>
--- a/src/schedule.xlsx
+++ b/src/schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Max\Documents\Master IIS\AMOS\amos2022ws01-firmware-scraper\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2D8ED0A-1CF2-4A0B-98EB-BF8933B9575D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9967C26B-89CA-4E28-94D2-4933FFDAE22F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16320" yWindow="6945" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -105,10 +105,10 @@
     <t>TPLinkScraper</t>
   </si>
   <si>
-    <t>Rockwell</t>
-  </si>
-  <si>
-    <t>RockwellScraper</t>
+    <t>Gigaset</t>
+  </si>
+  <si>
+    <t>GigasetScraper</t>
   </si>
 </sst>
 </file>
@@ -183,7 +183,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -207,6 +207,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -515,7 +518,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -550,75 +553,76 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="B2" s="7">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="C2" s="6">
-        <v>44934</v>
+        <v>44894</v>
       </c>
       <c r="D2" s="6">
-        <v>44935</v>
-      </c>
-      <c r="E2" t="s">
-        <v>27</v>
+        <v>44993</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" s="4">
         <v>100</v>
       </c>
       <c r="C3" s="5">
-        <v>44894</v>
+        <v>44893</v>
       </c>
       <c r="D3" s="6">
-        <v>44993</v>
+        <v>45261</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4" s="4">
         <v>100</v>
       </c>
       <c r="C4" s="5">
-        <v>44893</v>
+        <v>44901</v>
       </c>
       <c r="D4" s="6">
         <v>45261</v>
       </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="7">
+        <v>10</v>
+      </c>
     </row>
     <row r="5" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B5" s="4">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="C5" s="5">
-        <v>44901</v>
+        <v>44902</v>
       </c>
       <c r="D5" s="6">
-        <v>44938</v>
+        <v>45261</v>
       </c>
       <c r="E5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="4">
-        <v>10</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B6" s="4">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="C6" s="5">
         <v>44902</v>
@@ -627,24 +631,24 @@
         <v>45261</v>
       </c>
       <c r="E6" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="B7" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="6">
-        <v>44902</v>
+        <v>44934</v>
       </c>
       <c r="D7" s="6">
-        <v>45261</v>
+        <v>44943</v>
       </c>
       <c r="E7" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -652,7 +656,7 @@
         <v>14</v>
       </c>
       <c r="B8" s="4">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="C8" s="6">
         <v>44902</v>
@@ -669,9 +673,9 @@
         <v>16</v>
       </c>
       <c r="B9" s="7">
-        <v>0</v>
-      </c>
-      <c r="C9" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="C9" s="9" t="s">
         <v>17</v>
       </c>
       <c r="D9" s="8">
@@ -686,9 +690,9 @@
         <v>19</v>
       </c>
       <c r="B10" s="7">
-        <v>0</v>
-      </c>
-      <c r="C10" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="C10" s="9" t="s">
         <v>20</v>
       </c>
       <c r="D10" s="8">
@@ -703,7 +707,7 @@
         <v>22</v>
       </c>
       <c r="B11" s="7">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="C11" s="8">
         <v>44902</v>

</xml_diff>